<commit_message>
feat: useInput hook create , uploadPage [중간저장]
</commit_message>
<xml_diff>
--- a/public/oneTest.xlsx
+++ b/public/oneTest.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>이름</t>
   </si>
@@ -25,7 +25,28 @@
     <t>회사명</t>
   </si>
   <si>
-    <t>할말</t>
+    <t>택배회사명</t>
+  </si>
+  <si>
+    <t>택배배송시간</t>
+  </si>
+  <si>
+    <t>송장번호</t>
+  </si>
+  <si>
+    <t>주문번호</t>
+  </si>
+  <si>
+    <t>구/면</t>
+  </si>
+  <si>
+    <t>동/리</t>
+  </si>
+  <si>
+    <t>배송예정일</t>
+  </si>
+  <si>
+    <t>결제금액</t>
   </si>
   <si>
     <t>김영현</t>
@@ -40,19 +61,35 @@
     <t>센딩고</t>
   </si>
   <si>
-    <t>보내지려나!</t>
+    <t>CJ택배</t>
+  </si>
+  <si>
+    <t>처인구</t>
+  </si>
+  <si>
+    <t>왕곡동</t>
+  </si>
+  <si>
+    <t>2일뒤</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="am/pm h:mm"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color theme="1"/>
@@ -74,14 +111,20 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -316,22 +359,64 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.5416666666666666</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2.901248912E9</v>
+      </c>
+      <c r="H2" s="2">
+        <v>912399.0</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="2">
+        <v>33000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>